<commit_message>
add ps4 controller diagram
</commit_message>
<xml_diff>
--- a/docs/drone_control/data-flow.xlsx
+++ b/docs/drone_control/data-flow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tmori/project/oss/hakoniwa-px4sim/docs/drone_control/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3026B2DA-62CD-0945-ADF5-59A87AB0123A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40F66139-E457-034B-A966-0F2C14F119FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-7660" yWindow="-28300" windowWidth="51200" windowHeight="26800" xr2:uid="{04AAAEE0-CBA9-B946-A6FA-4BC89A99C738}"/>
   </bookViews>
@@ -903,16 +903,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>145132</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>657229</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>72879</xdr:rowOff>
+      <xdr:rowOff>83121</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>877497</xdr:colOff>
+      <xdr:colOff>437094</xdr:colOff>
       <xdr:row>25</xdr:row>
-      <xdr:rowOff>153821</xdr:rowOff>
+      <xdr:rowOff>164063</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -927,7 +927,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8604971" y="5705944"/>
+          <a:off x="8164568" y="5716186"/>
           <a:ext cx="1684865" cy="849087"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -990,13 +990,13 @@
       <xdr:col>4</xdr:col>
       <xdr:colOff>758965</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>244261</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>145132</xdr:colOff>
+      <xdr:rowOff>246379</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>657229</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>246379</xdr:rowOff>
+      <xdr:rowOff>251617</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1013,9 +1013,9 @@
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
-        <a:xfrm flipV="1">
-          <a:off x="4456304" y="6133374"/>
-          <a:ext cx="4148667" cy="2118"/>
+        <a:xfrm>
+          <a:off x="4456304" y="6135492"/>
+          <a:ext cx="3708264" cy="5238"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1043,16 +1043,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>111266</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>725783</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>136383</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>77399</xdr:colOff>
-      <xdr:row>24</xdr:row>
-      <xdr:rowOff>210397</xdr:rowOff>
+      <xdr:rowOff>208077</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>225323</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>26042</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1067,8 +1067,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="17143605" y="5769448"/>
-          <a:ext cx="1871133" cy="586110"/>
+          <a:off x="10138122" y="5841142"/>
+          <a:ext cx="1404540" cy="586110"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1115,15 +1115,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>877497</xdr:colOff>
+      <xdr:colOff>437094</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>174414</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>111266</xdr:colOff>
+      <xdr:rowOff>245084</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>725783</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>244261</xdr:rowOff>
+      <xdr:rowOff>251617</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -1141,8 +1141,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="10289836" y="6063527"/>
-          <a:ext cx="6853769" cy="69847"/>
+          <a:off x="9849433" y="6134197"/>
+          <a:ext cx="288689" cy="6533"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -1910,16 +1910,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>64698</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>791875</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>210393</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>1199</xdr:colOff>
+      <xdr:rowOff>220635</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>728376</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>235794</xdr:rowOff>
+      <xdr:rowOff>246036</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1934,7 +1934,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8524537" y="6867651"/>
+          <a:off x="8299214" y="6877893"/>
           <a:ext cx="1841501" cy="537498"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2006,15 +2006,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>73164</xdr:colOff>
-      <xdr:row>30</xdr:row>
-      <xdr:rowOff>140611</xdr:rowOff>
+      <xdr:colOff>257519</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>79160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>9665</xdr:colOff>
-      <xdr:row>32</xdr:row>
-      <xdr:rowOff>162288</xdr:rowOff>
+      <xdr:colOff>194020</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>100836</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2029,7 +2029,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8533003" y="7822063"/>
+          <a:off x="8717358" y="8016660"/>
           <a:ext cx="1841501" cy="533773"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2107,13 +2107,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>521898</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>223093</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>64698</xdr:colOff>
+      <xdr:rowOff>233336</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>791875</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>81345</xdr:rowOff>
+      <xdr:rowOff>79483</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2131,8 +2131,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="8029237" y="7136399"/>
-          <a:ext cx="495300" cy="626398"/>
+          <a:off x="8029237" y="7146642"/>
+          <a:ext cx="269977" cy="614293"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2163,13 +2163,13 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>521898</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>81345</xdr:rowOff>
+      <xdr:rowOff>79483</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>73164</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>153311</xdr:rowOff>
+      <xdr:colOff>257519</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>89999</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2187,8 +2187,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8029237" y="7762797"/>
-          <a:ext cx="503766" cy="328014"/>
+          <a:off x="8029237" y="7760935"/>
+          <a:ext cx="688121" cy="522612"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2273,15 +2273,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>479564</xdr:colOff>
+      <xdr:colOff>715129</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>72879</xdr:rowOff>
+      <xdr:rowOff>83120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>263665</xdr:colOff>
+      <xdr:colOff>499230</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>153822</xdr:rowOff>
+      <xdr:rowOff>164063</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -2296,7 +2296,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10844403" y="7242234"/>
+          <a:off x="11079968" y="7252475"/>
           <a:ext cx="1689101" cy="849088"/>
         </a:xfrm>
         <a:prstGeom prst="roundRect">
@@ -2363,9 +2363,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>371615</xdr:colOff>
+      <xdr:colOff>607180</xdr:colOff>
       <xdr:row>28</xdr:row>
-      <xdr:rowOff>72879</xdr:rowOff>
+      <xdr:rowOff>83120</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2384,7 +2384,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11672791" y="3523821"/>
-          <a:ext cx="16163" cy="3718413"/>
+          <a:ext cx="251728" cy="3728654"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2412,16 +2412,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>728376</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>233336</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>1199</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>223093</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>479564</xdr:colOff>
+      <xdr:colOff>715129</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>244262</xdr:rowOff>
+      <xdr:rowOff>251616</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2439,8 +2439,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="10366038" y="7136399"/>
-          <a:ext cx="478365" cy="533266"/>
+          <a:off x="10140715" y="7146642"/>
+          <a:ext cx="939253" cy="530377"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2469,15 +2469,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>9665</xdr:colOff>
+      <xdr:colOff>194020</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>244262</xdr:rowOff>
+      <xdr:rowOff>251616</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>11</xdr:col>
-      <xdr:colOff>479564</xdr:colOff>
-      <xdr:row>31</xdr:row>
-      <xdr:rowOff>153311</xdr:rowOff>
+      <xdr:colOff>715129</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>89999</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2495,8 +2495,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="10374504" y="7669665"/>
-          <a:ext cx="469899" cy="421146"/>
+          <a:off x="10558859" y="7677019"/>
+          <a:ext cx="521109" cy="606528"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2695,15 +2695,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>263665</xdr:colOff>
+      <xdr:colOff>499230</xdr:colOff>
       <xdr:row>27</xdr:row>
-      <xdr:rowOff>214627</xdr:rowOff>
+      <xdr:rowOff>214628</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>703931</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>244262</xdr:rowOff>
+      <xdr:rowOff>251616</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2721,8 +2721,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm flipV="1">
-          <a:off x="12533504" y="7127933"/>
-          <a:ext cx="440266" cy="541732"/>
+          <a:off x="12769069" y="7127934"/>
+          <a:ext cx="204701" cy="549085"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -2751,15 +2751,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>263665</xdr:colOff>
+      <xdr:colOff>499230</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>244262</xdr:rowOff>
+      <xdr:rowOff>251616</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>763197</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>102510</xdr:rowOff>
+      <xdr:rowOff>102511</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -2777,8 +2777,8 @@
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12533504" y="7669665"/>
-          <a:ext cx="499532" cy="370345"/>
+          <a:off x="12769069" y="7677019"/>
+          <a:ext cx="263967" cy="362992"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -3974,16 +3974,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>77399</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>225323</xdr:colOff>
       <xdr:row>23</xdr:row>
-      <xdr:rowOff>173390</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>146906</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>74540</xdr:rowOff>
+      <xdr:rowOff>183632</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>22</xdr:col>
+      <xdr:colOff>36839</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>67144</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -3995,16 +3995,15 @@
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="24" idx="3"/>
-          <a:endCxn id="284" idx="1"/>
+          <a:endCxn id="284" idx="0"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="19014738" y="6062503"/>
-          <a:ext cx="1022007" cy="1437440"/>
-        </a:xfrm>
-        <a:prstGeom prst="straightConnector1">
+          <a:off x="11542662" y="6072745"/>
+          <a:ext cx="9336516" cy="907705"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector2">
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
@@ -4148,10 +4147,10 @@
       <xdr:rowOff>194597</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>35065</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>547162</xdr:colOff>
       <xdr:row>22</xdr:row>
-      <xdr:rowOff>72879</xdr:rowOff>
+      <xdr:rowOff>83121</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
@@ -4170,7 +4169,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8633259" y="3523226"/>
-          <a:ext cx="814145" cy="2182718"/>
+          <a:ext cx="373742" cy="2192960"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
           <a:avLst/>
@@ -4886,6 +4885,1008 @@
           <a:ext cx="3874942" cy="1321673"/>
         </a:xfrm>
         <a:prstGeom prst="bentConnector2">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>378952</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>102414</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>225319</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="角丸四角形 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{23763520-1325-A441-B584-9072B1036348}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4076291" y="9064108"/>
+          <a:ext cx="7241048" cy="1403146"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800" b="1">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+            </a:rPr>
+            <a:t>Radio</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800" b="1" baseline="0">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800" b="1">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+            </a:rPr>
+            <a:t>Control</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800" b="1">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>225769</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>100836</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>239888</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="21" name="直線矢印コネクタ 20">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4415186E-1366-254C-80DD-3674054CA8BB}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="87" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9694325" y="8482836"/>
+          <a:ext cx="14119" cy="1042164"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>19254</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>310444</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>183444</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="27" name="直線矢印コネクタ 26">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{228ED327-6FB9-F14A-805F-185B96E796CE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8528254" y="7366000"/>
+          <a:ext cx="291190" cy="2215444"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>857375</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>12203</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>793876</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>33878</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="51" name="正方形/長方形 50">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2E8FC8F7-24C9-2448-92CB-A8376CD37F73}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4554714" y="9485993"/>
+          <a:ext cx="1841501" cy="533772"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1100" b="1" i="1">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+            </a:rPr>
+            <a:t>Target Altitude</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100" b="1" i="1">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>825626</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>115213</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>835165</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>12203</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="52" name="直線矢印コネクタ 51">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{313E6026-05EE-FE4E-A223-5F0EA64A886F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:stCxn id="51" idx="0"/>
+          <a:endCxn id="64" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5475465" y="5492229"/>
+          <a:ext cx="9539" cy="3993764"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>322643</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>42333</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>783531</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>225778</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="63" name="角丸四角形 62">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42EEDA97-869E-134F-AB5F-4315C065C12D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4033865" y="10964333"/>
+          <a:ext cx="7177777" cy="1707445"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="lt1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="b"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr kumimoji="1" lang="en-US" altLang="ja-JP" sz="1800" b="1">
+              <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+              <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+            </a:rPr>
+            <a:t>PS4 Controller(Python)</a:t>
+          </a:r>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1800" b="1">
+            <a:latin typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+            <a:ea typeface="Meiryo UI" panose="020B0604030504040204" pitchFamily="34" charset="-128"/>
+          </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>475554</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>26042</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>479778</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>197556</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="454" name="直線矢印コネクタ 453">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2B2E99B-69B9-6E44-AA86-81D46F545B2F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="24" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="10903665" y="6376042"/>
+          <a:ext cx="4224" cy="3473514"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>467259</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>52347</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>160001</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>183444</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="457" name="円/楕円 456">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8740C990-0956-4F68-41E5-80E0D9BCA2BD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5138037" y="11482347"/>
+          <a:ext cx="652297" cy="639097"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>711835</xdr:colOff>
+      <xdr:row>45</xdr:row>
+      <xdr:rowOff>212940</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>404577</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>92086</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="458" name="円/楕円 457">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{39E6AC81-EC1A-BF48-A4A8-7E8E72F098D3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9220835" y="11642940"/>
+          <a:ext cx="652298" cy="641146"/>
+        </a:xfrm>
+        <a:prstGeom prst="ellipse">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1">
+            <a:shade val="15000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="l"/>
+          <a:endParaRPr kumimoji="1" lang="ja-JP" altLang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>795001</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>214169</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>795001</xdr:colOff>
+      <xdr:row>49</xdr:row>
+      <xdr:rowOff>175250</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="460" name="直線矢印コネクタ 459">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7889C28-04D2-C6D5-F0B2-8B3080B70248}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5465779" y="11136169"/>
+          <a:ext cx="0" cy="1485081"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>834740</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>112569</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>856453</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>113798</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="461" name="直線矢印コネクタ 460">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F643A1E5-B73C-4648-9058-4FDE82B62929}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4545962" y="11796569"/>
+          <a:ext cx="1940824" cy="1229"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>87078</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>81844</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>87078</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>40877</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="463" name="直線矢印コネクタ 462">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C7B9E69-B538-3843-8B68-DB028087397E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="9555634" y="11257844"/>
+          <a:ext cx="0" cy="1483033"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>126817</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>232196</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>148530</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>233425</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="464" name="直線矢印コネクタ 463">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1767AE1-D076-6F42-9AED-89371621A8B1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8635817" y="11916196"/>
+          <a:ext cx="1940824" cy="1229"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle" w="med" len="med"/>
+          <a:tailEnd type="triangle" w="med" len="med"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>804333</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>33878</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>825625</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>225778</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="465" name="直線矢印コネクタ 464">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45D1F1A8-9B7C-C240-987E-F506E80C891A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr>
+          <a:endCxn id="51" idx="2"/>
+        </xdr:cNvCxnSpPr>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="5475111" y="9939878"/>
+          <a:ext cx="21292" cy="1207900"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>493889</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>239889</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>479778</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>42333</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="470" name="直線矢印コネクタ 469">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{390EC0AB-52F7-1146-A43F-D7B3F48797F5}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipV="1">
+          <a:off x="6124222" y="9891889"/>
+          <a:ext cx="4783667" cy="1834444"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>282222</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>239889</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>84666</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>169333</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="476" name="直線矢印コネクタ 475">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E9AAD3F-D62F-8147-A0E3-93158B926EC8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="8791222" y="9637889"/>
+          <a:ext cx="762000" cy="1707444"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="dk1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="dk1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="dk1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>239888</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>169333</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>733777</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>28222</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="478" name="直線矢印コネクタ 477">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5A68CBB1-D99B-4A47-9D96-29AB67E54377}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm flipH="1" flipV="1">
+          <a:off x="9708444" y="9567333"/>
+          <a:ext cx="493889" cy="2398889"/>
+        </a:xfrm>
+        <a:prstGeom prst="straightConnector1">
           <a:avLst/>
         </a:prstGeom>
         <a:ln>
@@ -5231,8 +6232,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CA5866C-C199-A54E-AB69-CAF0AEF3B7A4}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="R34" sqref="R34"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="D49" sqref="D49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20"/>

</xml_diff>